<commit_message>
updated steel plant data
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Steel Plant Data Full.xlsx
+++ b/mppsteel/data/import_data/Steel Plant Data Full.xlsx
@@ -7695,8 +7695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3794053-1996-4A5D-8AE8-E83BBC7AD429}">
   <dimension ref="A1:Y610"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -57475,6 +57475,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
+      <UserInfo>
+        <DisplayName>Min Guan</DisplayName>
+        <AccountId>24316</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
@@ -57691,30 +57714,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F1C171-0731-4E67-B6D0-DAF52E056163}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
-      <UserInfo>
-        <DisplayName>Min Guan</DisplayName>
-        <AccountId>24316</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE718BC2-02D3-4116-9C84-8BCFE1E3BEF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D616CAE8-17C5-45C5-A280-8DDE7D6EB953}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -57731,22 +57749,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE718BC2-02D3-4116-9C84-8BCFE1E3BEF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F1C171-0731-4E67-B6D0-DAF52E056163}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>